<commit_message>
roadmap.csv updates and test -- updated gitignore to allow the lastest roadmap outputs
</commit_message>
<xml_diff>
--- a/roadmap.xlsx
+++ b/roadmap.xlsx
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -338,6 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -708,7 +709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB42"/>
+  <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
@@ -2147,15 +2148,15 @@
       <c r="B34" s="18" t="n"/>
       <c r="C34" s="9" t="inlineStr">
         <is>
-          <t>Tenant X PROD (RMF 0-3)</t>
+          <t>HSM DEV Account Setup</t>
         </is>
       </c>
       <c r="D34" s="18" t="n"/>
-      <c r="E34" s="59" t="inlineStr"/>
-      <c r="F34" s="60" t="inlineStr"/>
+      <c r="E34" s="18" t="n"/>
+      <c r="F34" s="28" t="n"/>
       <c r="G34" s="59" t="inlineStr"/>
-      <c r="H34" s="18" t="n"/>
-      <c r="I34" s="18" t="n"/>
+      <c r="H34" s="59" t="inlineStr"/>
+      <c r="I34" s="59" t="inlineStr"/>
       <c r="J34" s="18" t="n"/>
       <c r="K34" s="18" t="n"/>
       <c r="L34" s="18" t="n"/>
@@ -2177,92 +2178,92 @@
       <c r="AB34" s="18" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="13" t="n"/>
-      <c r="B35" s="13" t="n"/>
-      <c r="C35" s="14" t="inlineStr">
-        <is>
-          <t>HSM DEV Account Setup</t>
-        </is>
-      </c>
-      <c r="D35" s="13" t="n"/>
-      <c r="E35" s="13" t="n"/>
-      <c r="F35" s="15" t="n"/>
-      <c r="G35" s="61" t="inlineStr"/>
-      <c r="H35" s="61" t="inlineStr"/>
-      <c r="I35" s="61" t="inlineStr"/>
-      <c r="J35" s="13" t="n"/>
-      <c r="K35" s="13" t="n"/>
-      <c r="L35" s="13" t="n"/>
-      <c r="M35" s="13" t="n"/>
-      <c r="N35" s="13" t="n"/>
-      <c r="O35" s="13" t="n"/>
-      <c r="P35" s="13" t="n"/>
-      <c r="Q35" s="13" t="n"/>
-      <c r="R35" s="13" t="n"/>
-      <c r="S35" s="13" t="n"/>
-      <c r="T35" s="13" t="n"/>
-      <c r="U35" s="13" t="n"/>
-      <c r="V35" s="13" t="n"/>
-      <c r="W35" s="13" t="n"/>
-      <c r="X35" s="13" t="n"/>
-      <c r="Y35" s="13" t="n"/>
-      <c r="Z35" s="13" t="n"/>
-      <c r="AA35" s="13" t="n"/>
-      <c r="AB35" s="13" t="n"/>
+      <c r="A35" s="18" t="n"/>
+      <c r="B35" s="18" t="n"/>
+      <c r="C35" s="9" t="inlineStr">
+        <is>
+          <t>HSM DEV Account Integration</t>
+        </is>
+      </c>
+      <c r="D35" s="18" t="n"/>
+      <c r="E35" s="18" t="n"/>
+      <c r="F35" s="28" t="n"/>
+      <c r="G35" s="18" t="n"/>
+      <c r="H35" s="18" t="n"/>
+      <c r="I35" s="59" t="inlineStr"/>
+      <c r="J35" s="59" t="inlineStr"/>
+      <c r="K35" s="59" t="inlineStr"/>
+      <c r="L35" s="59" t="inlineStr"/>
+      <c r="M35" s="59" t="inlineStr"/>
+      <c r="N35" s="18" t="n"/>
+      <c r="O35" s="18" t="n"/>
+      <c r="P35" s="18" t="n"/>
+      <c r="Q35" s="18" t="n"/>
+      <c r="R35" s="18" t="n"/>
+      <c r="S35" s="18" t="n"/>
+      <c r="T35" s="18" t="n"/>
+      <c r="U35" s="18" t="n"/>
+      <c r="V35" s="18" t="n"/>
+      <c r="W35" s="18" t="n"/>
+      <c r="X35" s="18" t="n"/>
+      <c r="Y35" s="18" t="n"/>
+      <c r="Z35" s="18" t="n"/>
+      <c r="AA35" s="18" t="n"/>
+      <c r="AB35" s="18" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="18" t="n"/>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>Tenant X PROD</t>
-        </is>
-      </c>
-      <c r="C36" s="9" t="inlineStr">
-        <is>
-          <t>Tenant X PROD Account Setup</t>
-        </is>
-      </c>
-      <c r="D36" s="18" t="n"/>
-      <c r="E36" s="18" t="n"/>
-      <c r="F36" s="28" t="n"/>
-      <c r="G36" s="62" t="inlineStr"/>
-      <c r="H36" s="62" t="inlineStr"/>
-      <c r="I36" s="62" t="inlineStr"/>
-      <c r="J36" s="18" t="n"/>
-      <c r="K36" s="18" t="n"/>
-      <c r="L36" s="18" t="n"/>
-      <c r="M36" s="18" t="n"/>
-      <c r="N36" s="18" t="n"/>
-      <c r="O36" s="18" t="n"/>
-      <c r="P36" s="18" t="n"/>
-      <c r="Q36" s="18" t="n"/>
-      <c r="R36" s="18" t="n"/>
-      <c r="S36" s="18" t="n"/>
-      <c r="T36" s="18" t="n"/>
-      <c r="U36" s="18" t="n"/>
-      <c r="V36" s="18" t="n"/>
-      <c r="W36" s="18" t="n"/>
-      <c r="X36" s="18" t="n"/>
-      <c r="Y36" s="18" t="n"/>
-      <c r="Z36" s="18" t="n"/>
-      <c r="AA36" s="18" t="n"/>
-      <c r="AB36" s="18" t="n"/>
+      <c r="A36" s="13" t="n"/>
+      <c r="B36" s="13" t="n"/>
+      <c r="C36" s="14" t="inlineStr">
+        <is>
+          <t>HSM Multi-Tenant Resource Cleanup</t>
+        </is>
+      </c>
+      <c r="D36" s="13" t="n"/>
+      <c r="E36" s="13" t="n"/>
+      <c r="F36" s="15" t="n"/>
+      <c r="G36" s="13" t="n"/>
+      <c r="H36" s="13" t="n"/>
+      <c r="I36" s="13" t="n"/>
+      <c r="J36" s="13" t="n"/>
+      <c r="K36" s="13" t="n"/>
+      <c r="L36" s="61" t="inlineStr"/>
+      <c r="M36" s="61" t="inlineStr"/>
+      <c r="N36" s="13" t="n"/>
+      <c r="O36" s="13" t="n"/>
+      <c r="P36" s="13" t="n"/>
+      <c r="Q36" s="13" t="n"/>
+      <c r="R36" s="13" t="n"/>
+      <c r="S36" s="13" t="n"/>
+      <c r="T36" s="13" t="n"/>
+      <c r="U36" s="13" t="n"/>
+      <c r="V36" s="13" t="n"/>
+      <c r="W36" s="13" t="n"/>
+      <c r="X36" s="13" t="n"/>
+      <c r="Y36" s="13" t="n"/>
+      <c r="Z36" s="13" t="n"/>
+      <c r="AA36" s="13" t="n"/>
+      <c r="AB36" s="13" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="18" t="n"/>
-      <c r="B37" s="18" t="n"/>
+      <c r="B37" s="8" t="inlineStr">
+        <is>
+          <t>Tenant X PROD</t>
+        </is>
+      </c>
       <c r="C37" s="9" t="inlineStr">
         <is>
-          <t>Tenant X PROD Account Integration</t>
+          <t>Tenant X PROD (RMF 0-3)</t>
         </is>
       </c>
       <c r="D37" s="18" t="n"/>
-      <c r="E37" s="18" t="n"/>
-      <c r="F37" s="28" t="n"/>
-      <c r="G37" s="18" t="n"/>
+      <c r="E37" s="62" t="inlineStr"/>
+      <c r="F37" s="63" t="inlineStr"/>
+      <c r="G37" s="62" t="inlineStr"/>
       <c r="H37" s="18" t="n"/>
-      <c r="I37" s="62" t="inlineStr"/>
-      <c r="J37" s="62" t="inlineStr"/>
+      <c r="I37" s="18" t="n"/>
+      <c r="J37" s="18" t="n"/>
       <c r="K37" s="18" t="n"/>
       <c r="L37" s="18" t="n"/>
       <c r="M37" s="18" t="n"/>
@@ -2283,63 +2284,131 @@
       <c r="AB37" s="18" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="41" t="n"/>
-      <c r="B38" s="41" t="n"/>
-      <c r="C38" s="42" t="inlineStr">
+      <c r="A38" s="18" t="n"/>
+      <c r="B38" s="18" t="n"/>
+      <c r="C38" s="9" t="inlineStr">
+        <is>
+          <t>Tenant X PROD Account Setup</t>
+        </is>
+      </c>
+      <c r="D38" s="18" t="n"/>
+      <c r="E38" s="18" t="n"/>
+      <c r="F38" s="28" t="n"/>
+      <c r="G38" s="62" t="inlineStr"/>
+      <c r="H38" s="62" t="inlineStr"/>
+      <c r="I38" s="62" t="inlineStr"/>
+      <c r="J38" s="18" t="n"/>
+      <c r="K38" s="18" t="n"/>
+      <c r="L38" s="18" t="n"/>
+      <c r="M38" s="18" t="n"/>
+      <c r="N38" s="18" t="n"/>
+      <c r="O38" s="18" t="n"/>
+      <c r="P38" s="18" t="n"/>
+      <c r="Q38" s="18" t="n"/>
+      <c r="R38" s="18" t="n"/>
+      <c r="S38" s="18" t="n"/>
+      <c r="T38" s="18" t="n"/>
+      <c r="U38" s="18" t="n"/>
+      <c r="V38" s="18" t="n"/>
+      <c r="W38" s="18" t="n"/>
+      <c r="X38" s="18" t="n"/>
+      <c r="Y38" s="18" t="n"/>
+      <c r="Z38" s="18" t="n"/>
+      <c r="AA38" s="18" t="n"/>
+      <c r="AB38" s="18" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="18" t="n"/>
+      <c r="B39" s="18" t="n"/>
+      <c r="C39" s="9" t="inlineStr">
+        <is>
+          <t>Tenant X PROD Account Integration</t>
+        </is>
+      </c>
+      <c r="D39" s="18" t="n"/>
+      <c r="E39" s="18" t="n"/>
+      <c r="F39" s="28" t="n"/>
+      <c r="G39" s="18" t="n"/>
+      <c r="H39" s="18" t="n"/>
+      <c r="I39" s="62" t="inlineStr"/>
+      <c r="J39" s="62" t="inlineStr"/>
+      <c r="K39" s="62" t="inlineStr"/>
+      <c r="L39" s="18" t="n"/>
+      <c r="M39" s="18" t="n"/>
+      <c r="N39" s="18" t="n"/>
+      <c r="O39" s="18" t="n"/>
+      <c r="P39" s="18" t="n"/>
+      <c r="Q39" s="18" t="n"/>
+      <c r="R39" s="18" t="n"/>
+      <c r="S39" s="18" t="n"/>
+      <c r="T39" s="18" t="n"/>
+      <c r="U39" s="18" t="n"/>
+      <c r="V39" s="18" t="n"/>
+      <c r="W39" s="18" t="n"/>
+      <c r="X39" s="18" t="n"/>
+      <c r="Y39" s="18" t="n"/>
+      <c r="Z39" s="18" t="n"/>
+      <c r="AA39" s="18" t="n"/>
+      <c r="AB39" s="18" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="41" t="n"/>
+      <c r="B40" s="41" t="n"/>
+      <c r="C40" s="42" t="inlineStr">
         <is>
           <t>Tenant X PROD ATO</t>
         </is>
       </c>
-      <c r="D38" s="41" t="n"/>
-      <c r="E38" s="41" t="n"/>
-      <c r="F38" s="43" t="n"/>
-      <c r="G38" s="41" t="n"/>
-      <c r="H38" s="41" t="n"/>
-      <c r="I38" s="63" t="inlineStr"/>
-      <c r="J38" s="63" t="inlineStr"/>
-      <c r="K38" s="63" t="inlineStr"/>
-      <c r="L38" s="41" t="n"/>
-      <c r="M38" s="41" t="n"/>
-      <c r="N38" s="41" t="n"/>
-      <c r="O38" s="41" t="n"/>
-      <c r="P38" s="41" t="n"/>
-      <c r="Q38" s="41" t="n"/>
-      <c r="R38" s="41" t="n"/>
-      <c r="S38" s="41" t="n"/>
-      <c r="T38" s="41" t="n"/>
-      <c r="U38" s="41" t="n"/>
-      <c r="V38" s="41" t="n"/>
-      <c r="W38" s="41" t="n"/>
-      <c r="X38" s="41" t="n"/>
-      <c r="Y38" s="41" t="n"/>
-      <c r="Z38" s="41" t="n"/>
-      <c r="AA38" s="41" t="n"/>
-      <c r="AB38" s="41" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="inlineStr">
+      <c r="D40" s="41" t="n"/>
+      <c r="E40" s="41" t="n"/>
+      <c r="F40" s="43" t="n"/>
+      <c r="G40" s="41" t="n"/>
+      <c r="H40" s="41" t="n"/>
+      <c r="I40" s="64" t="inlineStr"/>
+      <c r="J40" s="64" t="inlineStr"/>
+      <c r="K40" s="64" t="inlineStr"/>
+      <c r="L40" s="41" t="n"/>
+      <c r="M40" s="41" t="n"/>
+      <c r="N40" s="41" t="n"/>
+      <c r="O40" s="41" t="n"/>
+      <c r="P40" s="41" t="n"/>
+      <c r="Q40" s="41" t="n"/>
+      <c r="R40" s="41" t="n"/>
+      <c r="S40" s="41" t="n"/>
+      <c r="T40" s="41" t="n"/>
+      <c r="U40" s="41" t="n"/>
+      <c r="V40" s="41" t="n"/>
+      <c r="W40" s="41" t="n"/>
+      <c r="X40" s="41" t="n"/>
+      <c r="Y40" s="41" t="n"/>
+      <c r="Z40" s="41" t="n"/>
+      <c r="AA40" s="41" t="n"/>
+      <c r="AB40" s="41" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>Legend:</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="64" t="inlineStr">
+    <row r="44">
+      <c r="A44" s="65" t="inlineStr">
         <is>
           <t>Baseline (primary offering)</t>
         </is>
       </c>
-      <c r="B42" s="65" t="inlineStr">
+      <c r="B44" s="66" t="inlineStr">
         <is>
           <t>Green left accent</t>
         </is>
       </c>
-      <c r="C42" s="66" t="inlineStr">
+      <c r="C44" s="67" t="inlineStr">
         <is>
           <t>Optional</t>
         </is>
       </c>
-      <c r="D42" s="65" t="inlineStr">
+      <c r="D44" s="66" t="inlineStr">
         <is>
           <t>Orange dashed left accent</t>
         </is>
@@ -2348,18 +2417,18 @@
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A4:A24"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B37:B40"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A33:A40"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2371,7 +2440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2389,37 +2458,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="67" t="inlineStr">
+      <c r="A1" s="68" t="inlineStr">
         <is>
           <t>domain</t>
         </is>
       </c>
-      <c r="B1" s="67" t="inlineStr">
+      <c r="B1" s="68" t="inlineStr">
         <is>
           <t>feature</t>
         </is>
       </c>
-      <c r="C1" s="67" t="inlineStr">
+      <c r="C1" s="68" t="inlineStr">
         <is>
           <t>task</t>
         </is>
       </c>
-      <c r="D1" s="67" t="inlineStr">
+      <c r="D1" s="68" t="inlineStr">
         <is>
           <t>start</t>
         </is>
       </c>
-      <c r="E1" s="67" t="inlineStr">
+      <c r="E1" s="68" t="inlineStr">
         <is>
           <t>end</t>
         </is>
       </c>
-      <c r="F1" s="67" t="inlineStr">
+      <c r="F1" s="68" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="G1" s="67" t="inlineStr">
+      <c r="G1" s="68" t="inlineStr">
         <is>
           <t>flag</t>
         </is>
@@ -3524,17 +3593,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tenant X PROD (RMF 0-3)</t>
+          <t>HSM DEV Account Setup</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Jan 2026</t>
+          <t>Mar 2026</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Mar 2026</t>
+          <t>May 2026</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -3557,17 +3626,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HSM DEV Account Setup</t>
+          <t>HSM DEV Account Integration</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mar 2026</t>
+          <t>May 2026</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>May 2026</t>
+          <t>Sep 2026</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -3585,22 +3654,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Tenant X PROD</t>
+          <t>HSM DEV</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tenant X PROD Account Setup</t>
+          <t>HSM Multi-Tenant Resource Cleanup</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Mar 2026</t>
+          <t>Aug 2026</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>May 2026</t>
+          <t>Sep 2026</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -3623,17 +3692,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Tenant X PROD Account Integration</t>
+          <t>Tenant X PROD (RMF 0-3)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>May 2026</t>
+          <t>Jan 2026</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Jun 2026</t>
+          <t>Mar 2026</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -3656,23 +3725,89 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Tenant X PROD ATO</t>
+          <t>Tenant X PROD Account Setup</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t>Mar 2026</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>May 2026</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Jul 2026</t>
         </is>
       </c>
       <c r="F36" t="n">
         <v/>
       </c>
       <c r="G36" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Onboarding Tenant Apps</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Tenant X PROD</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Tenant X PROD Account Integration</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>May 2026</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Jul 2026</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v/>
+      </c>
+      <c r="G37" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Onboarding Tenant Apps</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Tenant X PROD</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Tenant X PROD ATO</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>May 2026</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Jul 2026</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v/>
+      </c>
+      <c r="G38" t="n">
         <v/>
       </c>
     </row>
@@ -3701,17 +3836,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="67" t="inlineStr">
+      <c r="A1" s="68" t="inlineStr">
         <is>
           <t>release</t>
         </is>
       </c>
-      <c r="B1" s="67" t="inlineStr">
+      <c r="B1" s="68" t="inlineStr">
         <is>
           <t>start</t>
         </is>
       </c>
-      <c r="C1" s="67" t="inlineStr">
+      <c r="C1" s="68" t="inlineStr">
         <is>
           <t>end</t>
         </is>

</xml_diff>